<commit_message>
Actualización de la ruta del archivo BASEABC.xlsx en unionBase.py y mejoras en la validación de datos en integral.py. Se eliminan archivos innecesarios y se ajusta el formato de salida de resultados.
</commit_message>
<xml_diff>
--- a/BASEABC.xlsx
+++ b/BASEABC.xlsx
@@ -1,26 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Juan\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Juan\Desktop\UDEA\Algo\ProyectoAlgo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{A7E43379-EC3A-490E-A80B-13FEA9641BFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40B082D7-22E5-4CE3-AE1B-53740BD4B01D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10140" yWindow="0" windowWidth="10455" windowHeight="10905" xr2:uid="{B446647C-00D5-4D26-9694-157C336E301D}"/>
   </bookViews>
   <sheets>
     <sheet name="BASEABC" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="79">
   <si>
     <t>Tipo de sustancia</t>
   </si>
@@ -61,111 +74,9 @@
     <t>l</t>
   </si>
   <si>
-    <t>K</t>
-  </si>
-  <si>
     <t>c</t>
   </si>
   <si>
-    <t>Cumeno (isopropilbenceno)</t>
-  </si>
-  <si>
-    <t>Dioxido de azufre</t>
-  </si>
-  <si>
-    <t>Dioxido de carbono</t>
-  </si>
-  <si>
-    <t>Dioxido de nitrogeno</t>
-  </si>
-  <si>
-    <t>Etano</t>
-  </si>
-  <si>
-    <t>Etileno</t>
-  </si>
-  <si>
-    <t>Formaldehido</t>
-  </si>
-  <si>
-    <t>Helio</t>
-  </si>
-  <si>
-    <t>n-Hexano</t>
-  </si>
-  <si>
-    <t>Hidrogeno</t>
-  </si>
-  <si>
-    <t>Hidroxido de calcio</t>
-  </si>
-  <si>
-    <t>Isobutano</t>
-  </si>
-  <si>
-    <t>Isbuteno</t>
-  </si>
-  <si>
-    <t>Metano</t>
-  </si>
-  <si>
-    <t>Metilciclohexano</t>
-  </si>
-  <si>
-    <t>Metilciclopentano</t>
-  </si>
-  <si>
-    <t>Mon—xido de carbono</t>
-  </si>
-  <si>
-    <t>Nitrogeno</t>
-  </si>
-  <si>
-    <t>Oxido de calcio</t>
-  </si>
-  <si>
-    <t>Oxido de magnesio</t>
-  </si>
-  <si>
-    <t>Oxido ferrico</t>
-  </si>
-  <si>
-    <t>Oxido nitrico</t>
-  </si>
-  <si>
-    <t>Oxido nitroso</t>
-  </si>
-  <si>
-    <t>Oxigeno</t>
-  </si>
-  <si>
-    <t>n-Pentano</t>
-  </si>
-  <si>
-    <t>propano</t>
-  </si>
-  <si>
-    <t>Propileno</t>
-  </si>
-  <si>
-    <t>Tetracloruro de carbono</t>
-  </si>
-  <si>
-    <t>Tetroxido de nitrogeno</t>
-  </si>
-  <si>
-    <t>Tolueno</t>
-  </si>
-  <si>
-    <t>Trioxido de azufre</t>
-  </si>
-  <si>
-    <t>Sulfato de amonio</t>
-  </si>
-  <si>
-    <t>Sulfuro de hidrogeno</t>
-  </si>
-  <si>
     <t>Acido nitrico l</t>
   </si>
   <si>
@@ -245,13 +156,130 @@
   </si>
   <si>
     <t>Cobre c</t>
+  </si>
+  <si>
+    <t>Celsius (°C)</t>
+  </si>
+  <si>
+    <t>Kelvin (K)</t>
+  </si>
+  <si>
+    <t>Cumeno (isopropilbenceno) g</t>
+  </si>
+  <si>
+    <t>Dioxido de azufre g</t>
+  </si>
+  <si>
+    <t>Dioxido de carbono g</t>
+  </si>
+  <si>
+    <t>Dioxido de nitrogeno g</t>
+  </si>
+  <si>
+    <t>Etano g</t>
+  </si>
+  <si>
+    <t>Etileno g</t>
+  </si>
+  <si>
+    <t>Formaldehido g</t>
+  </si>
+  <si>
+    <t>Helio g</t>
+  </si>
+  <si>
+    <t>n-Hexano l</t>
+  </si>
+  <si>
+    <t>n-Hexano g</t>
+  </si>
+  <si>
+    <t>Hidrogeno g</t>
+  </si>
+  <si>
+    <t>Hidroxido de calcio g</t>
+  </si>
+  <si>
+    <t>Isobutano g</t>
+  </si>
+  <si>
+    <t>Isbuteno g</t>
+  </si>
+  <si>
+    <t>Metano g</t>
+  </si>
+  <si>
+    <t>Metilciclohexano g</t>
+  </si>
+  <si>
+    <t>Metilciclopentano g</t>
+  </si>
+  <si>
+    <t>Nitrogeno g</t>
+  </si>
+  <si>
+    <t>Oxido de calcio c</t>
+  </si>
+  <si>
+    <t>Oxido de magnesio c</t>
+  </si>
+  <si>
+    <t>Oxido ferrico c</t>
+  </si>
+  <si>
+    <t>Oxido nitrico g</t>
+  </si>
+  <si>
+    <t>Oxido nitroso g</t>
+  </si>
+  <si>
+    <t>Oxigeno g</t>
+  </si>
+  <si>
+    <t>n-Pentano l</t>
+  </si>
+  <si>
+    <t>n-Pentano g</t>
+  </si>
+  <si>
+    <t>propano g</t>
+  </si>
+  <si>
+    <t>Propileno g</t>
+  </si>
+  <si>
+    <t>Monoxido de carbono g</t>
+  </si>
+  <si>
+    <t>Tetracloruro de carbono l</t>
+  </si>
+  <si>
+    <t>Tetroxido de nitrogeno g</t>
+  </si>
+  <si>
+    <t>Tolueno l</t>
+  </si>
+  <si>
+    <t>Tolueno g</t>
+  </si>
+  <si>
+    <t>Trioxido de azufre g</t>
+  </si>
+  <si>
+    <t>Sulfato de amonio c</t>
+  </si>
+  <si>
+    <t>Sulfuro de hidrogeno g</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="169" formatCode="#,##0.000"/>
+  </numFmts>
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -382,6 +410,28 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="24"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -728,9 +778,30 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1106,18 +1177,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E73459BF-E23E-4CA8-A6A3-EEA8F1B53143}">
-  <dimension ref="A1:L71"/>
+  <dimension ref="A1:Q71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1152,11 +1223,14 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
         <f>_xlfn.CONCAT("Acetileno ",D2)</f>
         <v>Acetileno g</v>
       </c>
+      <c r="C2">
+        <v>26.04</v>
+      </c>
       <c r="D2" t="s">
         <v>11</v>
       </c>
@@ -1164,7 +1238,7 @@
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="G2">
         <v>42.43</v>
@@ -1184,12 +1258,16 @@
       <c r="L2">
         <v>1200</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O2" s="3"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
         <f>_xlfn.CONCAT("Acetona ", D3)</f>
         <v>Acetona l</v>
       </c>
+      <c r="C3">
+        <v>58.08</v>
+      </c>
       <c r="D3" t="s">
         <v>12</v>
       </c>
@@ -1197,7 +1275,7 @@
         <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="G3">
         <v>123</v>
@@ -1205,6 +1283,12 @@
       <c r="H3">
         <v>18.600000000000001</v>
       </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
       <c r="K3">
         <v>-30</v>
       </c>
@@ -1212,11 +1296,14 @@
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
         <f>_xlfn.CONCAT("Acetona ", D4)</f>
         <v>Acetona g</v>
       </c>
+      <c r="C4">
+        <v>58.08</v>
+      </c>
       <c r="D4" t="s">
         <v>11</v>
       </c>
@@ -1224,7 +1311,7 @@
         <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="G4">
         <v>71.959999999999994</v>
@@ -1244,10 +1331,16 @@
       <c r="L4">
         <v>1200</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O4" s="4"/>
+      <c r="P4" s="4"/>
+      <c r="Q4" s="4"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>48</v>
+        <v>14</v>
+      </c>
+      <c r="C5">
+        <v>63.02</v>
       </c>
       <c r="D5" t="s">
         <v>12</v>
@@ -1256,21 +1349,36 @@
         <v>1</v>
       </c>
       <c r="F5" t="s">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="G5">
         <v>110</v>
       </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
       <c r="K5">
         <v>25</v>
       </c>
       <c r="L5">
         <v>25</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O5" s="5"/>
+      <c r="P5" s="5"/>
+      <c r="Q5" s="5"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>49</v>
+        <v>15</v>
+      </c>
+      <c r="C6">
+        <v>98.08</v>
       </c>
       <c r="D6" t="s">
         <v>12</v>
@@ -1279,7 +1387,7 @@
         <v>1</v>
       </c>
       <c r="F6" t="s">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="G6">
         <v>139.1</v>
@@ -1287,16 +1395,28 @@
       <c r="H6">
         <v>15.59</v>
       </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
       <c r="K6">
         <v>10</v>
       </c>
       <c r="L6">
         <v>45</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O6" s="5"/>
+      <c r="P6" s="5"/>
+      <c r="Q6" s="5"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>50</v>
+        <v>16</v>
+      </c>
+      <c r="C7" s="10">
+        <v>18.015999999999998</v>
       </c>
       <c r="D7" t="s">
         <v>12</v>
@@ -1305,21 +1425,36 @@
         <v>1</v>
       </c>
       <c r="F7" t="s">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="G7">
         <v>75.400000000000006</v>
       </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
       <c r="K7">
         <v>0</v>
       </c>
       <c r="L7">
         <v>100</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O7" s="5"/>
+      <c r="P7" s="5"/>
+      <c r="Q7" s="5"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>51</v>
+        <v>17</v>
+      </c>
+      <c r="C8" s="10">
+        <v>18.015999999999998</v>
       </c>
       <c r="D8" t="s">
         <v>11</v>
@@ -1328,7 +1463,7 @@
         <v>1</v>
       </c>
       <c r="F8" t="s">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="G8">
         <v>33.46</v>
@@ -1348,10 +1483,16 @@
       <c r="L8">
         <v>1500</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O8" s="5"/>
+      <c r="P8" s="5"/>
+      <c r="Q8" s="5"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>52</v>
+        <v>18</v>
+      </c>
+      <c r="C9">
+        <v>29</v>
       </c>
       <c r="D9" t="s">
         <v>11</v>
@@ -1360,7 +1501,7 @@
         <v>1</v>
       </c>
       <c r="F9" t="s">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="G9">
         <v>28.94</v>
@@ -1371,7 +1512,7 @@
       <c r="I9">
         <v>0.31909999999999999</v>
       </c>
-      <c r="J9">
+      <c r="J9" s="2">
         <v>-1.9650000000000001</v>
       </c>
       <c r="K9">
@@ -1380,10 +1521,16 @@
       <c r="L9">
         <v>1500</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O9" s="5"/>
+      <c r="P9" s="5"/>
+      <c r="Q9" s="5"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>52</v>
+        <v>18</v>
+      </c>
+      <c r="C10">
+        <v>29</v>
       </c>
       <c r="D10" t="s">
         <v>11</v>
@@ -1392,7 +1539,7 @@
         <v>1</v>
       </c>
       <c r="F10" t="s">
-        <v>13</v>
+        <v>42</v>
       </c>
       <c r="G10">
         <v>28.09</v>
@@ -1412,10 +1559,16 @@
       <c r="L10">
         <v>1800</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O10" s="5"/>
+      <c r="P10" s="5"/>
+      <c r="Q10" s="5"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>53</v>
+        <v>19</v>
+      </c>
+      <c r="C11">
+        <v>46.07</v>
       </c>
       <c r="D11" t="s">
         <v>12</v>
@@ -1424,21 +1577,36 @@
         <v>1</v>
       </c>
       <c r="F11" t="s">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="G11">
         <v>103.1</v>
       </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
       <c r="K11">
         <v>0</v>
       </c>
       <c r="L11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O11" s="5"/>
+      <c r="P11" s="5"/>
+      <c r="Q11" s="5"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>53</v>
+        <v>19</v>
+      </c>
+      <c r="C12">
+        <v>46.07</v>
       </c>
       <c r="D12" t="s">
         <v>12</v>
@@ -1447,18 +1615,36 @@
         <v>1</v>
       </c>
       <c r="F12" t="s">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="G12">
         <v>158.80000000000001</v>
       </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
       <c r="K12">
         <v>100</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L12">
+        <v>100</v>
+      </c>
+      <c r="O12" s="5"/>
+      <c r="P12" s="5"/>
+      <c r="Q12" s="5"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>54</v>
+        <v>20</v>
+      </c>
+      <c r="C13">
+        <v>46.07</v>
       </c>
       <c r="D13" t="s">
         <v>11</v>
@@ -1467,7 +1653,7 @@
         <v>1</v>
       </c>
       <c r="F13" t="s">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="G13">
         <v>61.34</v>
@@ -1487,10 +1673,16 @@
       <c r="L13">
         <v>1200</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O13" s="5"/>
+      <c r="P13" s="5"/>
+      <c r="Q13" s="5"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>55</v>
+        <v>21</v>
+      </c>
+      <c r="C14">
+        <v>32.04</v>
       </c>
       <c r="D14" t="s">
         <v>12</v>
@@ -1499,7 +1691,7 @@
         <v>1</v>
       </c>
       <c r="F14" t="s">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="G14">
         <v>75.86</v>
@@ -1513,10 +1705,16 @@
       <c r="L14">
         <v>65</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O14" s="5"/>
+      <c r="P14" s="5"/>
+      <c r="Q14" s="5"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>56</v>
+        <v>22</v>
+      </c>
+      <c r="C15">
+        <v>32.04</v>
       </c>
       <c r="D15" t="s">
         <v>11</v>
@@ -1525,7 +1723,7 @@
         <v>1</v>
       </c>
       <c r="F15" t="s">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="G15">
         <v>42.93</v>
@@ -1545,10 +1743,16 @@
       <c r="L15">
         <v>700</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O15" s="5"/>
+      <c r="P15" s="5"/>
+      <c r="Q15" s="5"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>57</v>
+        <v>23</v>
+      </c>
+      <c r="C16">
+        <v>17.03</v>
       </c>
       <c r="D16" t="s">
         <v>11</v>
@@ -1557,7 +1761,7 @@
         <v>1</v>
       </c>
       <c r="F16" t="s">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="G16">
         <v>35.15</v>
@@ -1577,19 +1781,25 @@
       <c r="L16">
         <v>1200</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O16" s="5"/>
+      <c r="P16" s="5"/>
+      <c r="Q16" s="5"/>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>58</v>
+        <v>24</v>
+      </c>
+      <c r="C17">
+        <v>32.07</v>
       </c>
       <c r="D17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E17">
         <v>1</v>
       </c>
       <c r="F17" t="s">
-        <v>13</v>
+        <v>42</v>
       </c>
       <c r="G17">
         <v>15.2</v>
@@ -1600,25 +1810,34 @@
       <c r="I17">
         <v>2.68</v>
       </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
       <c r="K17">
         <v>273</v>
       </c>
       <c r="L17">
         <v>368</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O17" s="5"/>
+      <c r="P17" s="5"/>
+      <c r="Q17" s="5"/>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>58</v>
+        <v>24</v>
+      </c>
+      <c r="C18">
+        <v>32.07</v>
       </c>
       <c r="D18" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E18">
         <v>1</v>
       </c>
       <c r="F18" t="s">
-        <v>13</v>
+        <v>42</v>
       </c>
       <c r="G18">
         <v>18.3</v>
@@ -1626,16 +1845,28 @@
       <c r="H18">
         <v>1.84</v>
       </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
       <c r="K18">
         <v>368</v>
       </c>
       <c r="L18">
         <v>392</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O18" s="5"/>
+      <c r="P18" s="5"/>
+      <c r="Q18" s="5"/>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>59</v>
+        <v>25</v>
+      </c>
+      <c r="C19" s="5">
+        <v>78.12</v>
       </c>
       <c r="D19" t="s">
         <v>12</v>
@@ -1644,7 +1875,7 @@
         <v>1</v>
       </c>
       <c r="F19" t="s">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="G19">
         <v>126.5</v>
@@ -1652,16 +1883,29 @@
       <c r="H19">
         <v>23.4</v>
       </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <v>0</v>
+      </c>
       <c r="K19">
         <v>6</v>
       </c>
       <c r="L19">
         <v>67</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O19" s="5"/>
+      <c r="P19" s="5"/>
+      <c r="Q19" s="5"/>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>60</v>
+        <v>26</v>
+      </c>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5">
+        <v>78.12</v>
       </c>
       <c r="D20" t="s">
         <v>11</v>
@@ -1670,7 +1914,7 @@
         <v>1</v>
       </c>
       <c r="F20" t="s">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="G20">
         <v>74.06</v>
@@ -1690,10 +1934,16 @@
       <c r="L20">
         <v>1200</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O20" s="5"/>
+      <c r="P20" s="5"/>
+      <c r="Q20" s="5"/>
+    </row>
+    <row r="21" spans="1:17" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>61</v>
+        <v>27</v>
+      </c>
+      <c r="C21" s="5">
+        <v>80.92</v>
       </c>
       <c r="D21" t="s">
         <v>11</v>
@@ -1702,7 +1952,7 @@
         <v>1</v>
       </c>
       <c r="F21" t="s">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="G21">
         <v>29.1</v>
@@ -1722,10 +1972,16 @@
       <c r="L21">
         <v>1200</v>
       </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O21" s="5"/>
+      <c r="P21" s="5"/>
+      <c r="Q21" s="5"/>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>62</v>
+        <v>28</v>
+      </c>
+      <c r="C22" s="5">
+        <v>58.12</v>
       </c>
       <c r="D22" t="s">
         <v>11</v>
@@ -1734,7 +1990,7 @@
         <v>1</v>
       </c>
       <c r="F22" t="s">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="G22">
         <v>92.3</v>
@@ -1754,19 +2010,25 @@
       <c r="L22">
         <v>1200</v>
       </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O22" s="5"/>
+      <c r="P22" s="5"/>
+      <c r="Q22" s="5"/>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>63</v>
+        <v>29</v>
+      </c>
+      <c r="C23" s="5">
+        <v>100.09</v>
       </c>
       <c r="D23" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E23">
         <v>2</v>
       </c>
       <c r="F23" t="s">
-        <v>13</v>
+        <v>42</v>
       </c>
       <c r="G23">
         <v>82.34</v>
@@ -1777,71 +2039,110 @@
       <c r="I23" s="1">
         <v>129000000000</v>
       </c>
+      <c r="J23">
+        <v>0</v>
+      </c>
       <c r="K23">
         <v>273</v>
       </c>
       <c r="L23">
         <v>1033</v>
       </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O23" s="5"/>
+      <c r="P23" s="5"/>
+      <c r="Q23" s="5"/>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>64</v>
+        <v>30</v>
+      </c>
+      <c r="C24" s="5">
+        <v>105.99</v>
       </c>
       <c r="D24" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E24">
         <v>1</v>
       </c>
       <c r="F24" t="s">
-        <v>13</v>
+        <v>42</v>
       </c>
       <c r="G24">
         <v>121</v>
       </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24">
+        <v>0</v>
+      </c>
+      <c r="J24">
+        <v>0</v>
+      </c>
       <c r="K24">
         <v>288</v>
       </c>
       <c r="L24">
         <v>371</v>
       </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O24" s="5"/>
+      <c r="P24" s="5"/>
+      <c r="Q24" s="5"/>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>65</v>
+        <v>31</v>
+      </c>
+      <c r="C25" s="5">
+        <v>286.14999999999998</v>
       </c>
       <c r="D25" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E25">
         <v>1</v>
       </c>
       <c r="F25" t="s">
-        <v>13</v>
+        <v>42</v>
       </c>
       <c r="G25">
         <v>535.6</v>
       </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+      <c r="I25">
+        <v>0</v>
+      </c>
+      <c r="J25">
+        <v>0</v>
+      </c>
       <c r="K25">
         <v>298</v>
       </c>
       <c r="L25">
         <v>298</v>
       </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O25" s="5"/>
+      <c r="P25" s="5"/>
+      <c r="Q25" s="5"/>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>66</v>
+        <v>32</v>
+      </c>
+      <c r="C26" s="5">
+        <v>12.01</v>
       </c>
       <c r="D26" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E26">
         <v>2</v>
       </c>
       <c r="F26" t="s">
-        <v>13</v>
+        <v>42</v>
       </c>
       <c r="G26">
         <v>11.18</v>
@@ -1852,25 +2153,34 @@
       <c r="I26" s="1">
         <v>-48900000000</v>
       </c>
+      <c r="J26">
+        <v>0</v>
+      </c>
       <c r="K26">
         <v>273</v>
       </c>
       <c r="L26">
         <v>-1373</v>
       </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O26" s="5"/>
+      <c r="P26" s="5"/>
+      <c r="Q26" s="5"/>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>67</v>
+        <v>33</v>
+      </c>
+      <c r="C27" s="5">
+        <v>64.099999999999994</v>
       </c>
       <c r="D27" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E27">
         <v>2</v>
       </c>
       <c r="F27" t="s">
-        <v>13</v>
+        <v>42</v>
       </c>
       <c r="G27">
         <v>68.62</v>
@@ -1881,16 +2191,25 @@
       <c r="I27" s="1">
         <v>-86600000000</v>
       </c>
+      <c r="J27">
+        <v>0</v>
+      </c>
       <c r="K27">
         <v>298</v>
       </c>
       <c r="L27">
         <v>720</v>
       </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O27" s="5"/>
+      <c r="P27" s="5"/>
+      <c r="Q27" s="5"/>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>68</v>
+        <v>34</v>
+      </c>
+      <c r="C28" s="5">
+        <v>27.03</v>
       </c>
       <c r="D28" t="s">
         <v>11</v>
@@ -1899,7 +2218,7 @@
         <v>1</v>
       </c>
       <c r="F28" t="s">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="G28">
         <v>35.299999999999997</v>
@@ -1910,16 +2229,25 @@
       <c r="I28">
         <v>1.0920000000000001</v>
       </c>
+      <c r="J28">
+        <v>0</v>
+      </c>
       <c r="K28">
         <v>0</v>
       </c>
       <c r="L28">
         <v>1200</v>
       </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O28" s="5"/>
+      <c r="P28" s="5"/>
+      <c r="Q28" s="5"/>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>69</v>
+        <v>35</v>
+      </c>
+      <c r="C29" s="5">
+        <v>84.16</v>
       </c>
       <c r="D29" t="s">
         <v>11</v>
@@ -1928,7 +2256,7 @@
         <v>1</v>
       </c>
       <c r="F29" t="s">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="G29">
         <v>94.14</v>
@@ -1948,10 +2276,16 @@
       <c r="L29">
         <v>1200</v>
       </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O29" s="5"/>
+      <c r="P29" s="5"/>
+      <c r="Q29" s="6"/>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>70</v>
+        <v>36</v>
+      </c>
+      <c r="C30" s="5">
+        <v>70.13</v>
       </c>
       <c r="D30" t="s">
         <v>11</v>
@@ -1960,7 +2294,7 @@
         <v>1</v>
       </c>
       <c r="F30" t="s">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="G30">
         <v>73.39</v>
@@ -1980,10 +2314,16 @@
       <c r="L30">
         <v>1200</v>
       </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O30" s="5"/>
+      <c r="P30" s="5"/>
+      <c r="Q30" s="5"/>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>71</v>
+        <v>37</v>
+      </c>
+      <c r="C31" s="5">
+        <v>70.91</v>
       </c>
       <c r="D31" t="s">
         <v>11</v>
@@ -1992,7 +2332,7 @@
         <v>1</v>
       </c>
       <c r="F31" t="s">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="G31">
         <v>33.6</v>
@@ -2012,10 +2352,16 @@
       <c r="L31">
         <v>1200</v>
       </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O31" s="5"/>
+      <c r="P31" s="5"/>
+      <c r="Q31" s="5"/>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>72</v>
+        <v>38</v>
+      </c>
+      <c r="C32" s="5">
+        <v>36.47</v>
       </c>
       <c r="D32" t="s">
         <v>11</v>
@@ -2024,7 +2370,7 @@
         <v>1</v>
       </c>
       <c r="F32" t="s">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="G32">
         <v>29.13</v>
@@ -2044,19 +2390,25 @@
       <c r="L32">
         <v>1200</v>
       </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O32" s="5"/>
+      <c r="P32" s="5"/>
+      <c r="Q32" s="5"/>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>73</v>
+        <v>39</v>
+      </c>
+      <c r="C33" s="5">
+        <v>95.23</v>
       </c>
       <c r="D33" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E33">
         <v>1</v>
       </c>
       <c r="F33" t="s">
-        <v>13</v>
+        <v>42</v>
       </c>
       <c r="G33">
         <v>72.400000000000006</v>
@@ -2064,25 +2416,37 @@
       <c r="H33">
         <v>-1.58</v>
       </c>
+      <c r="I33">
+        <v>0</v>
+      </c>
+      <c r="J33">
+        <v>0</v>
+      </c>
       <c r="K33">
         <v>273</v>
       </c>
       <c r="L33">
         <v>991</v>
       </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O33" s="5"/>
+      <c r="P33" s="5"/>
+      <c r="Q33" s="5"/>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>74</v>
+        <v>40</v>
+      </c>
+      <c r="C34" s="5">
+        <v>63.54</v>
       </c>
       <c r="D34" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E34">
         <v>1</v>
       </c>
       <c r="F34" t="s">
-        <v>13</v>
+        <v>42</v>
       </c>
       <c r="G34">
         <v>22.76</v>
@@ -2090,22 +2454,37 @@
       <c r="H34">
         <v>0.61170000000000002</v>
       </c>
+      <c r="I34">
+        <v>0</v>
+      </c>
+      <c r="J34">
+        <v>0</v>
+      </c>
       <c r="K34">
         <v>273</v>
       </c>
       <c r="L34">
         <v>1357</v>
       </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O34" s="5"/>
+      <c r="P34" s="5"/>
+      <c r="Q34" s="5"/>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>15</v>
+        <v>43</v>
+      </c>
+      <c r="C35" s="5">
+        <v>120.19</v>
+      </c>
+      <c r="D35" t="s">
+        <v>11</v>
       </c>
       <c r="E35">
         <v>1</v>
       </c>
       <c r="F35" t="s">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="G35">
         <v>139.19999999999999</v>
@@ -2125,16 +2504,25 @@
       <c r="L35">
         <v>1200</v>
       </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O35" s="5"/>
+      <c r="P35" s="5"/>
+      <c r="Q35" s="5"/>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>16</v>
+        <v>44</v>
+      </c>
+      <c r="C36" s="5">
+        <v>64.069999999999993</v>
+      </c>
+      <c r="D36" t="s">
+        <v>11</v>
       </c>
       <c r="E36">
         <v>1</v>
       </c>
       <c r="F36" t="s">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="G36">
         <v>38.909999999999997</v>
@@ -2154,16 +2542,25 @@
       <c r="L36">
         <v>1500</v>
       </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O36" s="5"/>
+      <c r="P36" s="5"/>
+      <c r="Q36" s="5"/>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>17</v>
+        <v>45</v>
+      </c>
+      <c r="C37" s="5">
+        <v>44.01</v>
+      </c>
+      <c r="D37" t="s">
+        <v>11</v>
       </c>
       <c r="E37">
         <v>1</v>
       </c>
       <c r="F37" t="s">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="G37">
         <v>36.11</v>
@@ -2183,16 +2580,25 @@
       <c r="L37">
         <v>1500</v>
       </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O37" s="5"/>
+      <c r="P37" s="5"/>
+      <c r="Q37" s="5"/>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>18</v>
+        <v>46</v>
+      </c>
+      <c r="C38" s="5">
+        <v>46.01</v>
+      </c>
+      <c r="D38" t="s">
+        <v>11</v>
       </c>
       <c r="E38">
         <v>1</v>
       </c>
       <c r="F38" t="s">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="G38">
         <v>36.07</v>
@@ -2212,16 +2618,25 @@
       <c r="L38">
         <v>1200</v>
       </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O38" s="5"/>
+      <c r="P38" s="5"/>
+      <c r="Q38" s="5"/>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>19</v>
+        <v>47</v>
+      </c>
+      <c r="C39" s="5">
+        <v>30.07</v>
+      </c>
+      <c r="D39" t="s">
+        <v>11</v>
       </c>
       <c r="E39">
         <v>1</v>
       </c>
       <c r="F39" t="s">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="G39">
         <v>49.37</v>
@@ -2241,16 +2656,25 @@
       <c r="L39">
         <v>1200</v>
       </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O39" s="5"/>
+      <c r="P39" s="5"/>
+      <c r="Q39" s="5"/>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>20</v>
+        <v>48</v>
+      </c>
+      <c r="C40" s="5">
+        <v>28.05</v>
+      </c>
+      <c r="D40" t="s">
+        <v>11</v>
       </c>
       <c r="E40">
         <v>1</v>
       </c>
       <c r="F40" t="s">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="G40">
         <v>40.75</v>
@@ -2270,16 +2694,25 @@
       <c r="L40">
         <v>1200</v>
       </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O40" s="5"/>
+      <c r="P40" s="5"/>
+      <c r="Q40" s="5"/>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>21</v>
+        <v>49</v>
+      </c>
+      <c r="C41" s="5">
+        <v>30.03</v>
+      </c>
+      <c r="D41" t="s">
+        <v>11</v>
       </c>
       <c r="E41">
         <v>1</v>
       </c>
       <c r="F41" t="s">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="G41">
         <v>34.28</v>
@@ -2299,30 +2732,54 @@
       <c r="L41">
         <v>1200</v>
       </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O41" s="5"/>
+      <c r="P41" s="5"/>
+      <c r="Q41" s="5"/>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>22</v>
+        <v>50</v>
+      </c>
+      <c r="C42" s="5">
+        <v>4</v>
+      </c>
+      <c r="D42" t="s">
+        <v>11</v>
       </c>
       <c r="E42">
         <v>1</v>
       </c>
       <c r="F42" t="s">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="G42">
         <v>20.8</v>
       </c>
+      <c r="H42">
+        <v>0</v>
+      </c>
+      <c r="I42">
+        <v>0</v>
+      </c>
+      <c r="J42">
+        <v>0</v>
+      </c>
       <c r="K42">
         <v>0</v>
       </c>
       <c r="L42">
         <v>1200</v>
       </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O42" s="5"/>
+      <c r="P42" s="5"/>
+      <c r="Q42" s="5"/>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>23</v>
+        <v>51</v>
+      </c>
+      <c r="C43" s="5">
+        <v>86.17</v>
       </c>
       <c r="D43" t="s">
         <v>12</v>
@@ -2331,19 +2788,37 @@
         <v>1</v>
       </c>
       <c r="F43" t="s">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="G43">
         <v>216.3</v>
       </c>
+      <c r="H43">
+        <v>0</v>
+      </c>
+      <c r="I43">
+        <v>0</v>
+      </c>
+      <c r="J43">
+        <v>0</v>
+      </c>
       <c r="K43">
         <v>20</v>
       </c>
       <c r="L43">
         <v>100</v>
       </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O43" s="5"/>
+      <c r="P43" s="5"/>
+      <c r="Q43" s="5"/>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>52</v>
+      </c>
+      <c r="C44" s="5">
+        <v>86.17</v>
+      </c>
       <c r="D44" t="s">
         <v>11</v>
       </c>
@@ -2351,7 +2826,7 @@
         <v>1</v>
       </c>
       <c r="F44" t="s">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="G44">
         <v>137.44</v>
@@ -2371,16 +2846,25 @@
       <c r="L44">
         <v>1200</v>
       </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O44" s="5"/>
+      <c r="P44" s="5"/>
+      <c r="Q44" s="5"/>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>24</v>
+        <v>53</v>
+      </c>
+      <c r="C45" s="8">
+        <v>2.016</v>
+      </c>
+      <c r="D45" t="s">
+        <v>11</v>
       </c>
       <c r="E45">
         <v>1</v>
       </c>
       <c r="F45" t="s">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="G45">
         <v>28.84</v>
@@ -2400,36 +2884,63 @@
       <c r="L45">
         <v>1500</v>
       </c>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O45" s="5"/>
+      <c r="P45" s="5"/>
+      <c r="Q45" s="5"/>
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>25</v>
+        <v>54</v>
+      </c>
+      <c r="C46" s="5">
+        <v>74.099999999999994</v>
+      </c>
+      <c r="D46" t="s">
+        <v>13</v>
       </c>
       <c r="E46">
         <v>1</v>
       </c>
       <c r="F46" t="s">
-        <v>13</v>
+        <v>42</v>
       </c>
       <c r="G46">
         <v>89.5</v>
       </c>
+      <c r="H46">
+        <v>0</v>
+      </c>
+      <c r="I46">
+        <v>0</v>
+      </c>
+      <c r="J46">
+        <v>0</v>
+      </c>
       <c r="K46">
         <v>276</v>
       </c>
       <c r="L46">
         <v>373</v>
       </c>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O46" s="5"/>
+      <c r="P46" s="5"/>
+      <c r="Q46" s="5"/>
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>26</v>
+        <v>55</v>
+      </c>
+      <c r="C47" s="5">
+        <v>58.12</v>
+      </c>
+      <c r="D47" t="s">
+        <v>11</v>
       </c>
       <c r="E47">
         <v>1</v>
       </c>
       <c r="F47" t="s">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="G47">
         <v>89.46</v>
@@ -2449,16 +2960,25 @@
       <c r="L47">
         <v>1200</v>
       </c>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O47" s="5"/>
+      <c r="P47" s="5"/>
+      <c r="Q47" s="5"/>
+    </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>27</v>
+        <v>56</v>
+      </c>
+      <c r="C48" s="9">
+        <v>56.1</v>
+      </c>
+      <c r="D48" t="s">
+        <v>11</v>
       </c>
       <c r="E48">
         <v>1</v>
       </c>
       <c r="F48" t="s">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="G48">
         <v>82.88</v>
@@ -2478,16 +2998,25 @@
       <c r="L48">
         <v>1200</v>
       </c>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O48" s="5"/>
+      <c r="P48" s="5"/>
+      <c r="Q48" s="5"/>
+    </row>
+    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>28</v>
+        <v>57</v>
+      </c>
+      <c r="C49" s="5">
+        <v>16.04</v>
+      </c>
+      <c r="D49" t="s">
+        <v>11</v>
       </c>
       <c r="E49">
         <v>1</v>
       </c>
       <c r="F49" t="s">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="G49">
         <v>34.31</v>
@@ -2507,13 +3036,25 @@
       <c r="L49">
         <v>1200</v>
       </c>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O49" s="5"/>
+      <c r="P49" s="5"/>
+      <c r="Q49" s="5"/>
+    </row>
+    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>57</v>
+      </c>
+      <c r="C50" s="5">
+        <v>16.04</v>
+      </c>
+      <c r="D50" t="s">
+        <v>11</v>
+      </c>
       <c r="E50">
         <v>1</v>
       </c>
       <c r="F50" t="s">
-        <v>13</v>
+        <v>42</v>
       </c>
       <c r="G50">
         <v>19.87</v>
@@ -2533,16 +3074,25 @@
       <c r="L50">
         <v>1500</v>
       </c>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O50" s="5"/>
+      <c r="P50" s="5"/>
+      <c r="Q50" s="5"/>
+    </row>
+    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>29</v>
+        <v>58</v>
+      </c>
+      <c r="C51" s="5">
+        <v>98.18</v>
+      </c>
+      <c r="D51" t="s">
+        <v>11</v>
       </c>
       <c r="E51">
         <v>1</v>
       </c>
       <c r="F51" t="s">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="G51">
         <v>121.3</v>
@@ -2562,16 +3112,25 @@
       <c r="L51">
         <v>1200</v>
       </c>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O51" s="5"/>
+      <c r="P51" s="5"/>
+      <c r="Q51" s="5"/>
+    </row>
+    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>30</v>
+        <v>59</v>
+      </c>
+      <c r="C52" s="5">
+        <v>84.16</v>
+      </c>
+      <c r="D52" t="s">
+        <v>11</v>
       </c>
       <c r="E52">
         <v>1</v>
       </c>
       <c r="F52" t="s">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="G52">
         <v>98.83</v>
@@ -2591,16 +3150,25 @@
       <c r="L52">
         <v>1200</v>
       </c>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O52" s="5"/>
+      <c r="P52" s="5"/>
+      <c r="Q52" s="5"/>
+    </row>
+    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>31</v>
+        <v>71</v>
+      </c>
+      <c r="C53" s="5">
+        <v>28.01</v>
+      </c>
+      <c r="D53" t="s">
+        <v>11</v>
       </c>
       <c r="E53">
         <v>1</v>
       </c>
       <c r="F53" t="s">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="G53">
         <v>28.95</v>
@@ -2621,15 +3189,21 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>32</v>
+        <v>60</v>
+      </c>
+      <c r="C54" s="5">
+        <v>28.02</v>
+      </c>
+      <c r="D54" t="s">
+        <v>11</v>
       </c>
       <c r="E54">
         <v>1</v>
       </c>
       <c r="F54" t="s">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="G54">
         <v>29</v>
@@ -2649,16 +3223,23 @@
       <c r="L54">
         <v>1500</v>
       </c>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="O54" s="7"/>
+    </row>
+    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>33</v>
+        <v>61</v>
+      </c>
+      <c r="C55" s="5">
+        <v>56.08</v>
+      </c>
+      <c r="D55" t="s">
+        <v>13</v>
       </c>
       <c r="E55">
         <v>2</v>
       </c>
       <c r="F55" t="s">
-        <v>13</v>
+        <v>42</v>
       </c>
       <c r="G55">
         <v>41.84</v>
@@ -2669,6 +3250,9 @@
       <c r="I55" s="1">
         <v>-45200000000</v>
       </c>
+      <c r="J55">
+        <v>0</v>
+      </c>
       <c r="K55">
         <v>273</v>
       </c>
@@ -2676,15 +3260,21 @@
         <v>1173</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>34</v>
+        <v>62</v>
+      </c>
+      <c r="C56" s="5">
+        <v>40.32</v>
+      </c>
+      <c r="D56" t="s">
+        <v>13</v>
       </c>
       <c r="E56">
         <v>2</v>
       </c>
       <c r="F56" t="s">
-        <v>13</v>
+        <v>42</v>
       </c>
       <c r="G56">
         <v>45.44</v>
@@ -2695,6 +3285,9 @@
       <c r="I56" s="1">
         <v>-87300000000</v>
       </c>
+      <c r="J56">
+        <v>0</v>
+      </c>
       <c r="K56">
         <v>273</v>
       </c>
@@ -2702,15 +3295,21 @@
         <v>2073</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>35</v>
+        <v>63</v>
+      </c>
+      <c r="C57" s="5">
+        <v>159.69999999999999</v>
+      </c>
+      <c r="D57" t="s">
+        <v>13</v>
       </c>
       <c r="E57">
         <v>2</v>
       </c>
       <c r="F57" t="s">
-        <v>13</v>
+        <v>42</v>
       </c>
       <c r="G57">
         <v>103.4</v>
@@ -2721,6 +3320,9 @@
       <c r="I57" s="1">
         <v>-177200000000</v>
       </c>
+      <c r="J57">
+        <v>0</v>
+      </c>
       <c r="K57">
         <v>273</v>
       </c>
@@ -2728,15 +3330,21 @@
         <v>1097</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>36</v>
+        <v>64</v>
+      </c>
+      <c r="C58" s="5">
+        <v>30.01</v>
+      </c>
+      <c r="D58" t="s">
+        <v>11</v>
       </c>
       <c r="E58">
         <v>1</v>
       </c>
       <c r="F58" t="s">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="G58">
         <v>29.5</v>
@@ -2757,15 +3365,21 @@
         <v>3500</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>37</v>
+        <v>65</v>
+      </c>
+      <c r="C59" s="5">
+        <v>44.02</v>
+      </c>
+      <c r="D59" t="s">
+        <v>11</v>
       </c>
       <c r="E59">
         <v>1</v>
       </c>
       <c r="F59" t="s">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="G59">
         <v>37.659999999999997</v>
@@ -2786,15 +3400,21 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>38</v>
+        <v>66</v>
+      </c>
+      <c r="C60" s="5">
+        <v>32</v>
+      </c>
+      <c r="D60" t="s">
+        <v>11</v>
       </c>
       <c r="E60">
         <v>1</v>
       </c>
       <c r="F60" t="s">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="G60">
         <v>29.1</v>
@@ -2815,15 +3435,21 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>39</v>
+        <v>67</v>
+      </c>
+      <c r="C61" s="5">
+        <v>72.150000000000006</v>
+      </c>
+      <c r="D61" t="s">
+        <v>12</v>
       </c>
       <c r="E61">
         <v>1</v>
       </c>
       <c r="F61" t="s">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="G61">
         <v>155.4</v>
@@ -2831,6 +3457,12 @@
       <c r="H61">
         <v>43.68</v>
       </c>
+      <c r="I61">
+        <v>0</v>
+      </c>
+      <c r="J61">
+        <v>0</v>
+      </c>
       <c r="K61">
         <v>0</v>
       </c>
@@ -2838,12 +3470,21 @@
         <v>36</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>68</v>
+      </c>
+      <c r="C62" s="5">
+        <v>72.150000000000006</v>
+      </c>
+      <c r="D62" t="s">
+        <v>11</v>
+      </c>
       <c r="E62">
         <v>1</v>
       </c>
       <c r="F62" t="s">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="G62">
         <v>114.8</v>
@@ -2864,15 +3505,21 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>40</v>
+        <v>69</v>
+      </c>
+      <c r="C63" s="5">
+        <v>44.09</v>
+      </c>
+      <c r="D63" t="s">
+        <v>11</v>
       </c>
       <c r="E63">
         <v>1</v>
       </c>
       <c r="F63" t="s">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="G63">
         <v>68.031999999999996</v>
@@ -2893,15 +3540,21 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>41</v>
+        <v>70</v>
+      </c>
+      <c r="C64" s="5">
+        <v>42.08</v>
+      </c>
+      <c r="D64" t="s">
+        <v>11</v>
       </c>
       <c r="E64">
         <v>1</v>
       </c>
       <c r="F64" t="s">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="G64">
         <v>59.58</v>
@@ -2924,13 +3577,19 @@
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
+        <v>72</v>
+      </c>
+      <c r="C65" s="5">
+        <v>153.84</v>
+      </c>
+      <c r="D65" t="s">
+        <v>12</v>
+      </c>
+      <c r="E65">
+        <v>1</v>
+      </c>
+      <c r="F65" t="s">
         <v>42</v>
-      </c>
-      <c r="E65">
-        <v>1</v>
-      </c>
-      <c r="F65" t="s">
-        <v>13</v>
       </c>
       <c r="G65">
         <v>93.39</v>
@@ -2938,6 +3597,12 @@
       <c r="H65">
         <v>12.98</v>
       </c>
+      <c r="I65">
+        <v>0</v>
+      </c>
+      <c r="J65">
+        <v>0</v>
+      </c>
       <c r="K65">
         <v>273</v>
       </c>
@@ -2947,13 +3612,19 @@
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>43</v>
+        <v>73</v>
+      </c>
+      <c r="C66" s="5">
+        <v>92.02</v>
+      </c>
+      <c r="D66" t="s">
+        <v>11</v>
       </c>
       <c r="E66">
         <v>1</v>
       </c>
       <c r="F66" t="s">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="G66">
         <v>75.7</v>
@@ -2964,6 +3635,9 @@
       <c r="I66">
         <v>-11.3</v>
       </c>
+      <c r="J66">
+        <v>0</v>
+      </c>
       <c r="K66">
         <v>0</v>
       </c>
@@ -2973,13 +3647,19 @@
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>44</v>
+        <v>74</v>
+      </c>
+      <c r="C67" s="5">
+        <v>92.13</v>
+      </c>
+      <c r="D67" t="s">
+        <v>12</v>
       </c>
       <c r="E67">
         <v>1</v>
       </c>
       <c r="F67" t="s">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="G67">
         <v>148.80000000000001</v>
@@ -2987,6 +3667,9 @@
       <c r="H67">
         <v>32.4</v>
       </c>
+      <c r="J67">
+        <v>0</v>
+      </c>
       <c r="K67">
         <v>0</v>
       </c>
@@ -2995,11 +3678,20 @@
       </c>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>75</v>
+      </c>
+      <c r="C68" s="5">
+        <v>92.13</v>
+      </c>
+      <c r="D68" t="s">
+        <v>11</v>
+      </c>
       <c r="E68">
         <v>1</v>
       </c>
       <c r="F68" t="s">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="G68">
         <v>94.18</v>
@@ -3022,13 +3714,19 @@
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>45</v>
+        <v>76</v>
+      </c>
+      <c r="C69" s="5">
+        <v>80.069999999999993</v>
+      </c>
+      <c r="D69" t="s">
+        <v>11</v>
       </c>
       <c r="E69">
         <v>1</v>
       </c>
       <c r="F69" t="s">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="G69">
         <v>48.5</v>
@@ -3051,17 +3749,32 @@
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>46</v>
+        <v>77</v>
+      </c>
+      <c r="C70" s="5">
+        <v>132.15</v>
+      </c>
+      <c r="D70" t="s">
+        <v>13</v>
       </c>
       <c r="E70">
         <v>1</v>
       </c>
       <c r="F70" t="s">
-        <v>13</v>
+        <v>42</v>
       </c>
       <c r="G70">
         <v>215.9</v>
       </c>
+      <c r="H70">
+        <v>0</v>
+      </c>
+      <c r="I70">
+        <v>0</v>
+      </c>
+      <c r="J70">
+        <v>0</v>
+      </c>
       <c r="K70">
         <v>275</v>
       </c>
@@ -3071,13 +3784,19 @@
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>47</v>
+        <v>78</v>
+      </c>
+      <c r="C71" s="5">
+        <v>34.08</v>
+      </c>
+      <c r="D71" t="s">
+        <v>11</v>
       </c>
       <c r="E71">
         <v>1</v>
       </c>
       <c r="F71" t="s">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="G71">
         <v>33.51</v>
@@ -3099,6 +3818,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="20" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>